<commit_message>
Fix lat/lon column names in Spanish template
</commit_message>
<xml_diff>
--- a/files/template-esp.xlsx
+++ b/files/template-esp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jryan\Documents\R\projects\soil-health-report-generator\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B30603D-6663-4273-81D2-9BBEC2FB1A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4ABD04-8C9D-4F25-8F1F-768049249D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -2406,7 +2406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB11E12-380E-4843-8FFB-3EEB7461C150}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2562,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2603,10 +2603,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>

</xml_diff>